<commit_message>
:construction: new method curves and excel sheet file generation
</commit_message>
<xml_diff>
--- a/src/results/methods-results.xlsx
+++ b/src/results/methods-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\awedi\OneDrive\Desktop\FSS\I2Semestre1\meta-heuristique\tp-meta-heuristique\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE8DBB42-678D-4555-AC31-6D51F9AC397C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB0903F5-A224-41D1-A7B9-8421D9430BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Méthode</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t>GA2</t>
-  </si>
-  <si>
-    <t>Meth ?</t>
-  </si>
-  <si>
-    <t>Meth ?.1</t>
   </si>
   <si>
     <t>MKP1</t>
@@ -66,6 +60,11 @@
 Écart type: 772967.48</t>
   </si>
   <si>
+    <t>Meilleure: -138998.00
+Moyenne: -141055.67
+Écart type: 772597.98</t>
+  </si>
+  <si>
     <t>MKP2</t>
   </si>
   <si>
@@ -89,6 +88,11 @@
 Écart type: 716231.79</t>
   </si>
   <si>
+    <t>Meilleure: -129173.00
+Moyenne: -130589.97
+Écart type: 715278.07</t>
+  </si>
+  <si>
     <t>MKP3</t>
   </si>
   <si>
@@ -112,6 +116,11 @@
 Écart type: 518533.85</t>
   </si>
   <si>
+    <t>Meilleure: -92958.00
+Moyenne: -94503.43
+Écart type: 517637.27</t>
+  </si>
+  <si>
     <t>MKP4</t>
   </si>
   <si>
@@ -135,6 +144,11 @@
 Écart type: 651695.27</t>
   </si>
   <si>
+    <t>Meilleure: -115831.00
+Moyenne: -118690.87
+Écart type: 650130.01</t>
+  </si>
+  <si>
     <t>MKP5</t>
   </si>
   <si>
@@ -158,6 +172,11 @@
 Écart type: 531640.22</t>
   </si>
   <si>
+    <t>Meilleure: -94348.00
+Moyenne: -96984.57
+Écart type: 531311.07</t>
+  </si>
+  <si>
     <t>MKP6</t>
   </si>
   <si>
@@ -181,6 +200,11 @@
 Écart type: 713967.94</t>
   </si>
   <si>
+    <t>Meilleure: -128273.00
+Moyenne: -130188.50
+Écart type: 713077.00</t>
+  </si>
+  <si>
     <t>MKP7</t>
   </si>
   <si>
@@ -204,6 +228,11 @@
 Écart type: 5998263.05</t>
   </si>
   <si>
+    <t>Meilleure: -1082340.00
+Moyenne: -1091400.87
+Écart type: 5977872.75</t>
+  </si>
+  <si>
     <t>MKP8</t>
   </si>
   <si>
@@ -227,6 +256,11 @@
 Écart type: 3393880.50</t>
   </si>
   <si>
+    <t>Meilleure: -536389.00
+Moyenne: -563492.13
+Écart type: 3087280.79</t>
+  </si>
+  <si>
     <t>MKP9</t>
   </si>
   <si>
@@ -250,6 +284,11 @@
 Écart type: 42505.32</t>
   </si>
   <si>
+    <t>Meilleure: -8782488147419108352.00
+Moyenne: -9095817368875833344.00
+Écart type: 49823197052037840896.00</t>
+  </si>
+  <si>
     <t>MKP10</t>
   </si>
   <si>
@@ -271,6 +310,14 @@
     <t>Meilleure: -8687.00
 Moyenne: -8711.43
 Écart type: 47714.52</t>
+  </si>
+  <si>
+    <t>Meilleure: -8609744073709557760.00
+Moyenne: -9106917690908452864.00
+Écart type: 49884316559818055680.00</t>
+  </si>
+  <si>
+    <t>HYBRID-BSO-GA1</t>
   </si>
 </sst>
 </file>
@@ -326,13 +373,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,20 +680,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="F2:G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="56.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="96.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,47 +708,50 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -722,124 +767,148 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:sparkles: new results generation
</commit_message>
<xml_diff>
--- a/src/results/methods-results.xlsx
+++ b/src/results/methods-results.xlsx
@@ -808,8 +808,8 @@
       <c r="G8" t="inlineStr">
         <is>
           <t>Meilleure: 1095445.00
-Moyenne: 1094958.43
-Écart type: 5997335.45</t>
+Moyenne: 1094931.07
+Écart type: 5997185.54</t>
         </is>
       </c>
     </row>
@@ -856,9 +856,9 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Meilleure: 623459.00
-Moyenne: 619645.33
-Écart type: 3393946.02</t>
+          <t>Meilleure: 624319.00
+Moyenne: 620104.20
+Écart type: 3396464.64</t>
         </is>
       </c>
     </row>
@@ -905,9 +905,9 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Meilleure: 9223232221128660992.00
-Moyenne: 9223043751676938240.00
-Écart type: 50516691145816989696.00</t>
+          <t>Meilleure: 7772.00
+Moyenne: 7760.37
+Écart type: 42505.32</t>
         </is>
       </c>
     </row>

</xml_diff>